<commit_message>
Update Register Account Test Case Script
</commit_message>
<xml_diff>
--- a/GithubPractice/Test_Document/TestCase_QAFOX.xlsx
+++ b/GithubPractice/Test_Document/TestCase_QAFOX.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="50">
   <si>
     <t>TestScenario_ID</t>
   </si>
@@ -139,6 +139,33 @@
   </si>
   <si>
     <t>Validate register account with valid Credentials</t>
+  </si>
+  <si>
+    <t>TS_03</t>
+  </si>
+  <si>
+    <t>Not fill lastname inputbox</t>
+  </si>
+  <si>
+    <t>Lastname  inputbox should be displayed empty</t>
+  </si>
+  <si>
+    <t>Error message should be displayed below blank mandatory filed (below Lastname inputbox because we should not fill lastname inputbox)</t>
+  </si>
+  <si>
+    <t>Validate Register Account Remains one mandatory field should be blank</t>
+  </si>
+  <si>
+    <t>TS_04</t>
+  </si>
+  <si>
+    <t>Validate Register account fill all fields but not select privacy policy Checkbox</t>
+  </si>
+  <si>
+    <t>Not Click privacy Policy checkbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">privacy policy checkbox should be displayed unchecked </t>
   </si>
 </sst>
 </file>
@@ -539,16 +566,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22.44140625" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="42.21875" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
@@ -641,7 +668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" ht="43.2">
+    <row r="10" spans="1:4" s="1" customFormat="1" ht="28.8">
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
@@ -697,7 +724,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="3:4" s="1" customFormat="1" ht="28.8">
+    <row r="17" spans="1:4" s="1" customFormat="1" ht="28.8">
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
@@ -705,7 +732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="3:4" s="1" customFormat="1" ht="28.8">
+    <row r="18" spans="1:4" s="1" customFormat="1" ht="28.8">
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
@@ -713,36 +740,245 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="3:4" s="1" customFormat="1"/>
-    <row r="20" spans="3:4" s="1" customFormat="1"/>
-    <row r="21" spans="3:4" s="1" customFormat="1"/>
-    <row r="22" spans="3:4" s="1" customFormat="1"/>
-    <row r="23" spans="3:4" s="1" customFormat="1"/>
-    <row r="24" spans="3:4" s="1" customFormat="1"/>
-    <row r="25" spans="3:4" s="1" customFormat="1"/>
-    <row r="26" spans="3:4" s="1" customFormat="1"/>
-    <row r="27" spans="3:4" s="1" customFormat="1"/>
-    <row r="28" spans="3:4" s="1" customFormat="1"/>
-    <row r="29" spans="3:4" s="1" customFormat="1"/>
-    <row r="30" spans="3:4" s="1" customFormat="1"/>
-    <row r="31" spans="3:4" s="1" customFormat="1"/>
-    <row r="32" spans="3:4" s="1" customFormat="1"/>
-    <row r="33" s="1" customFormat="1"/>
-    <row r="34" s="1" customFormat="1"/>
-    <row r="35" s="1" customFormat="1"/>
-    <row r="36" s="1" customFormat="1"/>
-    <row r="37" s="1" customFormat="1"/>
-    <row r="38" s="1" customFormat="1"/>
-    <row r="39" s="1" customFormat="1"/>
-    <row r="40" s="1" customFormat="1"/>
-    <row r="41" s="1" customFormat="1"/>
-    <row r="42" s="1" customFormat="1"/>
-    <row r="43" s="1" customFormat="1"/>
-    <row r="44" s="1" customFormat="1"/>
-    <row r="45" s="1" customFormat="1"/>
-    <row r="46" s="1" customFormat="1"/>
-    <row r="47" s="1" customFormat="1"/>
-    <row r="48" s="1" customFormat="1"/>
+    <row r="19" spans="1:4" s="1" customFormat="1"/>
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="A20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="1" customFormat="1">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="1" customFormat="1" ht="25.2" customHeight="1">
+      <c r="C24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="23.4" customHeight="1">
+      <c r="C28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="A34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="1" customFormat="1" ht="27" customHeight="1">
+      <c r="C35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="1" customFormat="1" ht="24" customHeight="1">
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C38" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="1" customFormat="1" ht="25.2" customHeight="1">
+      <c r="C39" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C41" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="1" customFormat="1" ht="23.4" customHeight="1">
+      <c r="C43" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="1" customFormat="1" ht="43.2">
+      <c r="C46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="1" customFormat="1" ht="28.8">
+      <c r="C48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="49" s="1" customFormat="1"/>
     <row r="50" s="1" customFormat="1"/>
     <row r="51" s="1" customFormat="1"/>
@@ -799,8 +1035,7 @@
     <row r="102" s="1" customFormat="1"/>
     <row r="103" s="1" customFormat="1"/>
     <row r="104" s="1" customFormat="1"/>
-    <row r="105" s="1" customFormat="1"/>
-    <row r="106" s="2" customFormat="1"/>
+    <row r="105" s="2" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>